<commit_message>
Figures and Improvements for Meeting
</commit_message>
<xml_diff>
--- a/rep100metrics.xlsx
+++ b/rep100metrics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="24440" yWindow="0" windowWidth="12720" windowHeight="12880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
   <si>
     <t>Divergence.Range</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>R0 = 7</t>
+  </si>
+  <si>
+    <t>MaxInfected</t>
   </si>
 </sst>
 </file>
@@ -113,8 +116,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -202,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -244,6 +249,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +291,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:I21"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -988,6 +995,69 @@
       </c>
       <c r="I21">
         <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>4.4180610000000002E-2</v>
+      </c>
+      <c r="B27">
+        <v>0.15590329999999999</v>
+      </c>
+      <c r="C27">
+        <v>0.27389229999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.35549989999999998</v>
+      </c>
+      <c r="E27">
+        <v>0.41962870000000002</v>
+      </c>
+      <c r="F27">
+        <v>0.46964280000000003</v>
+      </c>
+      <c r="G27">
+        <v>0.51334049999999998</v>
+      </c>
+      <c r="H27">
+        <v>0.54596710000000004</v>
+      </c>
+      <c r="I27">
+        <v>0.57680920000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>